<commit_message>
Feat: Model answers and update evaluation scores
</commit_message>
<xml_diff>
--- a/evaluations/Blood-Analysis-Gemma-bert-scores.xlsx
+++ b/evaluations/Blood-Analysis-Gemma-bert-scores.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rahul Sharma\OneDrive - UWA\Desktop\coroner\evaluations\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65021E6-CABC-419E-BB66-A53FFE729807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>FILENAME</t>
   </si>
@@ -171,8 +177,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +190,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,13 +247,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +299,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -313,6 +333,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -347,9 +368,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -522,14 +544,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:H11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -572,16 +596,22 @@
         <v>30</v>
       </c>
       <c r="F2">
-        <v>0.8749303221702576</v>
+        <v>0.87493032217025757</v>
       </c>
       <c r="G2">
         <v>0.8853422999382019</v>
       </c>
       <c r="H2">
-        <v>0.8801055550575256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+        <v>0.88010555505752563</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
@@ -595,13 +625,19 @@
         <v>0.8671841025352478</v>
       </c>
       <c r="G3">
-        <v>0.8647627830505371</v>
+        <v>0.86476278305053711</v>
       </c>
       <c r="H3">
-        <v>0.8659717440605164</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>0.86597174406051636</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -612,16 +648,22 @@
         <v>32</v>
       </c>
       <c r="F4">
-        <v>0.9217354655265808</v>
+        <v>0.92173546552658081</v>
       </c>
       <c r="G4">
         <v>0.8922463059425354</v>
       </c>
       <c r="H4">
-        <v>0.9067511558532715</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8">
+        <v>0.90675115585327148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
@@ -632,16 +674,22 @@
         <v>33</v>
       </c>
       <c r="F5">
-        <v>0.7876334190368652</v>
+        <v>0.78763341903686523</v>
       </c>
       <c r="G5">
-        <v>0.8063660264015198</v>
+        <v>0.80636602640151978</v>
       </c>
       <c r="H5">
-        <v>0.7968896627426147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.79688966274261475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
       <c r="C6" t="s">
         <v>14</v>
       </c>
@@ -652,16 +700,22 @@
         <v>34</v>
       </c>
       <c r="F6">
-        <v>0.9309383034706116</v>
+        <v>0.93093830347061157</v>
       </c>
       <c r="G6">
         <v>0.8821258544921875</v>
       </c>
       <c r="H6">
-        <v>0.905875027179718</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <v>0.90587502717971802</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
@@ -675,13 +729,19 @@
         <v>0.8528597354888916</v>
       </c>
       <c r="G7">
-        <v>0.8266919851303101</v>
+        <v>0.82669198513031006</v>
       </c>
       <c r="H7">
-        <v>0.839572012424469</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>0.83957201242446899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
@@ -692,16 +752,22 @@
         <v>36</v>
       </c>
       <c r="F8">
-        <v>0.8218851089477539</v>
+        <v>0.82188510894775391</v>
       </c>
       <c r="G8">
-        <v>0.8783594965934753</v>
+        <v>0.87835949659347534</v>
       </c>
       <c r="H8">
-        <v>0.8491843938827515</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <v>0.84918439388275146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
@@ -712,16 +778,22 @@
         <v>37</v>
       </c>
       <c r="F9">
-        <v>0.8801454901695251</v>
+        <v>0.88014549016952515</v>
       </c>
       <c r="G9">
-        <v>0.853946328163147</v>
+        <v>0.85394632816314697</v>
       </c>
       <c r="H9">
-        <v>0.8668479919433594</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <v>0.86684799194335938</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
       <c r="C10" t="s">
         <v>18</v>
       </c>
@@ -732,16 +804,22 @@
         <v>38</v>
       </c>
       <c r="F10">
-        <v>0.7878786325454712</v>
+        <v>0.78787863254547119</v>
       </c>
       <c r="G10">
-        <v>0.8411571979522705</v>
+        <v>0.84115719795227051</v>
       </c>
       <c r="H10">
-        <v>0.813646674156189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.81364667415618896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
@@ -752,16 +830,17 @@
         <v>39</v>
       </c>
       <c r="F11">
-        <v>0.830528736114502</v>
+        <v>0.83052873611450195</v>
       </c>
       <c r="G11">
-        <v>0.8923276662826538</v>
+        <v>0.89232766628265381</v>
       </c>
       <c r="H11">
-        <v>0.8603198528289795</v>
+        <v>0.86031985282897949</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>